<commit_message>
small fix for heating and TES storage
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/TIMES_DH_Demand_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/TIMES_DH_Demand_2050.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10459618_polimi_it/Documents/Università/Tesi (OneDrive)/Article PROres1 coupling/JRC-EU-TIMES Data/PROres/PROres Postprocessed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\JRC_EU_TIMES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B1EB7DC-F389-46F1-B251-AA53BE80A27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF27A6C-445C-4E06-AB22-8090C4303873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{01F8D9DD-8AB7-498F-A386-8002ED9D0540}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01F8D9DD-8AB7-498F-A386-8002ED9D0540}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -512,7 +514,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>50.971999999999994</v>
+        <v>56.891999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +550,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>4.9139999999999988</v>
+        <v>16.177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>11.699</v>
+        <v>29.441000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>13.809999999999999</v>
+        <v>15.66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>0.64400000000000002</v>
+        <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +582,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>45.045000000000002</v>
+        <v>103.03399999999999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>293.87700000000001</v>
+        <v>478.25199999999995</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>83.122</v>
+        <v>106.63600000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>16.090999999999998</v>
+        <v>20.350000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>1.238</v>
+        <v>3.1429999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +622,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>7.0750000000000002</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>94.790999999999997</v>
+        <v>118.413</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>106.97599999999998</v>
+        <v>140.54899999999998</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>6.9179999999999993</v>
+        <v>9.7460000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,21 +654,23 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>19.913999999999998</v>
+        <v>29.109000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="2">
+        <v>0.61899999999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>10.339000000000002</v>
+        <v>112.07000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,7 +678,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>17.663</v>
+        <v>33.222000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +686,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>1.119</v>
+        <v>1.885</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +694,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>18.13</v>
+        <v>22.69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +702,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>0.311</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +710,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>37.296999999999997</v>
+        <v>151.94999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +718,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>16.164999999999999</v>
+        <v>33.256</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +726,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>119.733</v>
+        <v>214.71400000000003</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +734,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>14.567</v>
+        <v>18.620999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +742,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>30.018999999999998</v>
+        <v>69.711000000000013</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,7 +750,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>129.63800000000001</v>
+        <v>146.411</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -754,7 +758,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <v>4.7229999999999999</v>
+        <v>7.6950000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,7 +766,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <v>18.927</v>
+        <v>26.805</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -770,7 +774,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <v>17.797999999999998</v>
+        <v>45.171000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>